<commit_message>
added standard regression plot to output
</commit_message>
<xml_diff>
--- a/quant_report.xlsx
+++ b/quant_report.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="quant_data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="quant_report" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="quant_standard" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="quant_report" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t xml:space="preserve">plate_id</t>
   </si>
@@ -124,6 +125,12 @@
   </si>
   <si>
     <t xml:space="preserve">O16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
   </si>
   <si>
     <t xml:space="preserve">sample_row</t>
@@ -246,6 +253,41 @@
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">12</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="5486400" cy="3657600"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="1" name="Picture 1"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -597,10 +639,10 @@
         <v>48.864</v>
       </c>
       <c r="J2" t="n">
-        <v>3.35459273426225</v>
+        <v>2.65639107083887</v>
       </c>
       <c r="K2" t="n">
-        <v>3.35459273426225</v>
+        <v>2.65639107083887</v>
       </c>
     </row>
     <row r="3">
@@ -632,10 +674,10 @@
         <v>98.035</v>
       </c>
       <c r="J3" t="n">
-        <v>6.73026151570481</v>
+        <v>5.69284555581591</v>
       </c>
       <c r="K3" t="n">
-        <v>6.73026151570481</v>
+        <v>5.69284555581591</v>
       </c>
     </row>
     <row r="4">
@@ -667,10 +709,10 @@
         <v>39.74</v>
       </c>
       <c r="J4" t="n">
-        <v>2.72821535812831</v>
+        <v>2.11849718139147</v>
       </c>
       <c r="K4" t="n">
-        <v>2.72821535812831</v>
+        <v>2.11849718139147</v>
       </c>
     </row>
     <row r="5">
@@ -702,10 +744,10 @@
         <v>43.964</v>
       </c>
       <c r="J5" t="n">
-        <v>3.0181997988111</v>
+        <v>2.36620799636509</v>
       </c>
       <c r="K5" t="n">
-        <v>3.0181997988111</v>
+        <v>2.36620799636509</v>
       </c>
     </row>
     <row r="6">
@@ -737,10 +779,10 @@
         <v>90.167</v>
       </c>
       <c r="J6" t="n">
-        <v>6.19011057363753</v>
+        <v>5.19462302180217</v>
       </c>
       <c r="K6" t="n">
-        <v>6.19011057363753</v>
+        <v>5.19462302180217</v>
       </c>
     </row>
     <row r="7">
@@ -772,10 +814,10 @@
         <v>60.913</v>
       </c>
       <c r="J7" t="n">
-        <v>4.18177609737468</v>
+        <v>3.38127521521168</v>
       </c>
       <c r="K7" t="n">
-        <v>4.18177609737468</v>
+        <v>3.38127521521168</v>
       </c>
     </row>
     <row r="8">
@@ -807,10 +849,10 @@
         <v>79.571</v>
       </c>
       <c r="J8" t="n">
-        <v>5.46267801362929</v>
+        <v>4.53020795243334</v>
       </c>
       <c r="K8" t="n">
-        <v>5.46267801362929</v>
+        <v>4.53020795243334</v>
       </c>
     </row>
     <row r="9">
@@ -842,10 +884,10 @@
         <v>40.911</v>
       </c>
       <c r="J9" t="n">
-        <v>2.80860640453919</v>
+        <v>2.18692991301082</v>
       </c>
       <c r="K9" t="n">
-        <v>2.80860640453919</v>
+        <v>2.18692991301082</v>
       </c>
     </row>
     <row r="10">
@@ -877,10 +919,10 @@
         <v>50.92</v>
       </c>
       <c r="J10" t="n">
-        <v>3.49574046391277</v>
+        <v>2.77898996517818</v>
       </c>
       <c r="K10" t="n">
-        <v>3.49574046391277</v>
+        <v>2.77898996517818</v>
       </c>
     </row>
     <row r="11">
@@ -912,10 +954,10 @@
         <v>102.102</v>
       </c>
       <c r="J11" t="n">
-        <v>7.00946765212926</v>
+        <v>5.95188806374297</v>
       </c>
       <c r="K11" t="n">
-        <v>7.00946765212926</v>
+        <v>5.95188806374297</v>
       </c>
     </row>
     <row r="12">
@@ -947,10 +989,10 @@
         <v>43.196</v>
       </c>
       <c r="J12" t="n">
-        <v>2.96547535505059</v>
+        <v>2.32099512424106</v>
       </c>
       <c r="K12" t="n">
-        <v>2.96547535505059</v>
+        <v>2.32099512424106</v>
       </c>
     </row>
     <row r="13">
@@ -982,10 +1024,10 @@
         <v>47.748</v>
       </c>
       <c r="J13" t="n">
-        <v>3.27797752692276</v>
+        <v>2.59004725984854</v>
       </c>
       <c r="K13" t="n">
-        <v>3.27797752692276</v>
+        <v>2.59004725984854</v>
       </c>
     </row>
     <row r="14">
@@ -1017,10 +1059,10 @@
         <v>99.175</v>
       </c>
       <c r="J14" t="n">
-        <v>6.80852436191181</v>
+        <v>5.76535556384493</v>
       </c>
       <c r="K14" t="n">
-        <v>6.80852436191181</v>
+        <v>5.76535556384493</v>
       </c>
     </row>
     <row r="15">
@@ -1052,10 +1094,10 @@
         <v>54.787</v>
       </c>
       <c r="J15" t="n">
-        <v>3.76121627644126</v>
+        <v>3.01083842728891</v>
       </c>
       <c r="K15" t="n">
-        <v>3.76121627644126</v>
+        <v>3.01083842728891</v>
       </c>
     </row>
     <row r="16">
@@ -1087,10 +1129,10 @@
         <v>65.575</v>
       </c>
       <c r="J16" t="n">
-        <v>4.50182994738963</v>
+        <v>3.66558112298234</v>
       </c>
       <c r="K16" t="n">
-        <v>4.50182994738963</v>
+        <v>3.66558112298234</v>
       </c>
     </row>
     <row r="17">
@@ -1122,10 +1164,10 @@
         <v>36.142</v>
       </c>
       <c r="J17" t="n">
-        <v>2.4812068312399</v>
+        <v>1.9094482659331</v>
       </c>
       <c r="K17" t="n">
-        <v>2.4812068312399</v>
+        <v>1.9094482659331</v>
       </c>
     </row>
   </sheetData>
@@ -1147,63 +1189,283 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.814</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>48.95</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>44.136</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.37634410119172</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>93.887</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>89.073</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5.12566580534331</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>180.096</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n">
+        <v>175.282</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10.7545185251621</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>336.554</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" t="n">
+        <v>331.74</v>
+      </c>
+      <c r="G6" t="n">
+        <v>21.6220620936095</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>441.693</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" t="n">
+        <v>436.879</v>
+      </c>
+      <c r="G7" t="n">
+        <v>29.2271543525334</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>507.526</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>40</v>
+      </c>
+      <c r="F8" t="n">
+        <v>502.712</v>
+      </c>
+      <c r="G8" t="n">
+        <v>34.0815316067401</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>759.432</v>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="n">
+        <v>754.618</v>
+      </c>
+      <c r="G9" t="n">
+        <v>53.1664821741219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C2" t="n">
         <v>12</v>
@@ -1227,10 +1489,10 @@
         <v>48.864</v>
       </c>
       <c r="J2" t="n">
-        <v>3.35459273426225</v>
+        <v>2.65639107083887</v>
       </c>
       <c r="K2" t="n">
-        <v>3.35459273426225</v>
+        <v>2.65639107083887</v>
       </c>
       <c r="L2" t="n">
         <v>55.734</v>
@@ -1239,19 +1501,19 @@
         <v>50.92</v>
       </c>
       <c r="N2" t="n">
-        <v>3.49574046391277</v>
+        <v>2.77898996517818</v>
       </c>
       <c r="O2" t="n">
-        <v>3.49574046391277</v>
+        <v>2.77898996517818</v>
       </c>
       <c r="P2" t="n">
-        <v>0.141147729650524</v>
+        <v>0.122598894339317</v>
       </c>
       <c r="Q2" t="n">
-        <v>3.42516659908751</v>
+        <v>2.71769051800853</v>
       </c>
       <c r="R2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -1259,7 +1521,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C3" t="n">
         <v>12</v>
@@ -1283,10 +1545,10 @@
         <v>98.035</v>
       </c>
       <c r="J3" t="n">
-        <v>6.73026151570481</v>
+        <v>5.69284555581591</v>
       </c>
       <c r="K3" t="n">
-        <v>6.73026151570481</v>
+        <v>5.69284555581591</v>
       </c>
       <c r="L3" t="n">
         <v>106.916</v>
@@ -1295,19 +1557,19 @@
         <v>102.102</v>
       </c>
       <c r="N3" t="n">
-        <v>7.00946765212926</v>
+        <v>5.95188806374297</v>
       </c>
       <c r="O3" t="n">
-        <v>7.00946765212926</v>
+        <v>5.95188806374297</v>
       </c>
       <c r="P3" t="n">
-        <v>0.279206136424455</v>
+        <v>0.259042507927067</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.86986458391704</v>
+        <v>5.82236680977944</v>
       </c>
       <c r="R3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
@@ -1315,7 +1577,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C4" t="n">
         <v>12</v>
@@ -1339,10 +1601,10 @@
         <v>39.74</v>
       </c>
       <c r="J4" t="n">
-        <v>2.72821535812831</v>
+        <v>2.11849718139147</v>
       </c>
       <c r="K4" t="n">
-        <v>2.72821535812831</v>
+        <v>2.11849718139147</v>
       </c>
       <c r="L4" t="n">
         <v>48.01</v>
@@ -1351,19 +1613,19 @@
         <v>43.196</v>
       </c>
       <c r="N4" t="n">
-        <v>2.96547535505059</v>
+        <v>2.32099512424106</v>
       </c>
       <c r="O4" t="n">
-        <v>2.96547535505059</v>
+        <v>2.32099512424106</v>
       </c>
       <c r="P4" t="n">
-        <v>0.237259996922281</v>
+        <v>0.202497942849586</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.84684535658945</v>
+        <v>2.21974615281626</v>
       </c>
       <c r="R4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -1371,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" t="n">
         <v>12</v>
@@ -1395,10 +1657,10 @@
         <v>43.964</v>
       </c>
       <c r="J5" t="n">
-        <v>3.0181997988111</v>
+        <v>2.36620799636509</v>
       </c>
       <c r="K5" t="n">
-        <v>3.0181997988111</v>
+        <v>2.36620799636509</v>
       </c>
       <c r="L5" t="n">
         <v>52.562</v>
@@ -1407,19 +1669,19 @@
         <v>47.748</v>
       </c>
       <c r="N5" t="n">
-        <v>3.27797752692276</v>
+        <v>2.59004725984854</v>
       </c>
       <c r="O5" t="n">
-        <v>3.27797752692276</v>
+        <v>2.59004725984854</v>
       </c>
       <c r="P5" t="n">
-        <v>0.259777728111664</v>
+        <v>0.223839263483446</v>
       </c>
       <c r="Q5" t="n">
-        <v>3.14808866286693</v>
+        <v>2.47812762810682</v>
       </c>
       <c r="R5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -1427,7 +1689,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" t="n">
         <v>12</v>
@@ -1451,10 +1713,10 @@
         <v>90.167</v>
       </c>
       <c r="J6" t="n">
-        <v>6.19011057363753</v>
+        <v>5.19462302180217</v>
       </c>
       <c r="K6" t="n">
-        <v>6.19011057363753</v>
+        <v>5.19462302180217</v>
       </c>
       <c r="L6" t="n">
         <v>103.989</v>
@@ -1463,19 +1725,19 @@
         <v>99.175</v>
       </c>
       <c r="N6" t="n">
-        <v>6.80852436191181</v>
+        <v>5.76535556384493</v>
       </c>
       <c r="O6" t="n">
-        <v>6.80852436191181</v>
+        <v>5.76535556384493</v>
       </c>
       <c r="P6" t="n">
-        <v>0.618413788274279</v>
+        <v>0.570732542042753</v>
       </c>
       <c r="Q6" t="n">
-        <v>6.49931746777467</v>
+        <v>5.47998929282355</v>
       </c>
       <c r="R6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
@@ -1483,7 +1745,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" t="n">
         <v>12</v>
@@ -1507,10 +1769,10 @@
         <v>60.913</v>
       </c>
       <c r="J7" t="n">
-        <v>4.18177609737468</v>
+        <v>3.38127521521168</v>
       </c>
       <c r="K7" t="n">
-        <v>4.18177609737468</v>
+        <v>3.38127521521168</v>
       </c>
       <c r="L7" t="n">
         <v>59.601</v>
@@ -1519,19 +1781,19 @@
         <v>54.787</v>
       </c>
       <c r="N7" t="n">
-        <v>3.76121627644126</v>
+        <v>3.01083842728891</v>
       </c>
       <c r="O7" t="n">
-        <v>3.76121627644126</v>
+        <v>3.01083842728891</v>
       </c>
       <c r="P7" t="n">
-        <v>0.420559820933418</v>
+        <v>0.370436787922773</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.97149618690797</v>
+        <v>3.19605682125029</v>
       </c>
       <c r="R7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
@@ -1539,7 +1801,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C8" t="n">
         <v>12</v>
@@ -1563,10 +1825,10 @@
         <v>79.571</v>
       </c>
       <c r="J8" t="n">
-        <v>5.46267801362929</v>
+        <v>4.53020795243334</v>
       </c>
       <c r="K8" t="n">
-        <v>5.46267801362929</v>
+        <v>4.53020795243334</v>
       </c>
       <c r="L8" t="n">
         <v>70.389</v>
@@ -1575,19 +1837,19 @@
         <v>65.575</v>
       </c>
       <c r="N8" t="n">
-        <v>4.50182994738963</v>
+        <v>3.66558112298234</v>
       </c>
       <c r="O8" t="n">
-        <v>4.50182994738963</v>
+        <v>3.66558112298234</v>
       </c>
       <c r="P8" t="n">
-        <v>0.960848066239655</v>
+        <v>0.864626829451008</v>
       </c>
       <c r="Q8" t="n">
-        <v>4.98225398050946</v>
+        <v>4.09789453770784</v>
       </c>
       <c r="R8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -1595,7 +1857,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C9" t="n">
         <v>12</v>
@@ -1619,10 +1881,10 @@
         <v>40.911</v>
       </c>
       <c r="J9" t="n">
-        <v>2.80860640453919</v>
+        <v>2.18692991301082</v>
       </c>
       <c r="K9" t="n">
-        <v>2.80860640453919</v>
+        <v>2.18692991301082</v>
       </c>
       <c r="L9" t="n">
         <v>40.956</v>
@@ -1631,19 +1893,19 @@
         <v>36.142</v>
       </c>
       <c r="N9" t="n">
-        <v>2.4812068312399</v>
+        <v>1.9094482659331</v>
       </c>
       <c r="O9" t="n">
-        <v>2.4812068312399</v>
+        <v>1.9094482659331</v>
       </c>
       <c r="P9" t="n">
-        <v>0.327399573299294</v>
+        <v>0.277481647077727</v>
       </c>
       <c r="Q9" t="n">
-        <v>2.64490661788954</v>
+        <v>2.04818908947196</v>
       </c>
       <c r="R9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>